<commit_message>
All function work properly
</commit_message>
<xml_diff>
--- a/BMI_Caculator Desktop App/Database.xlsx
+++ b/BMI_Caculator Desktop App/Database.xlsx
@@ -9,6 +9,8 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Peerapat" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Wiwat" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Chanakarn" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Jedilok" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -432,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,6 +599,69 @@
       <c r="E8" t="inlineStr">
         <is>
           <t>ผอม</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04/10/2021 21:45</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>50</v>
+      </c>
+      <c r="C9" t="n">
+        <v>170</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ผอม</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04/10/2021 21:45</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>80</v>
+      </c>
+      <c r="C10" t="n">
+        <v>170</v>
+      </c>
+      <c r="D10" t="n">
+        <v>27.68</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>อ้วน</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04/10/2021 21:46</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>100</v>
+      </c>
+      <c r="C11" t="n">
+        <v>170</v>
+      </c>
+      <c r="D11" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>อ้วนมาก</t>
         </is>
       </c>
     </row>
@@ -761,4 +826,131 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Chanakarn</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>เวลา</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>น้ำหนัก(กก.)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ส่วนสูง(ซม.)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>เกณฑ์</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>04/10/2021 21:46</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>170</v>
+      </c>
+      <c r="D3" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>อ้วนมาก</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Jedilok</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>เวลา</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>น้ำหนัก(กก.)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ส่วนสูง(ซม.)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>เกณฑ์</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>